<commit_message>
week 4 day 1
</commit_message>
<xml_diff>
--- a/User Stories/ASDE_Training_USER_STORIES - 2023.xlsx
+++ b/User Stories/ASDE_Training_USER_STORIES - 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online Training\ACE\Sapient\ASDE 2023\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E48EED-3213-4FA0-A3D3-AF05831D0D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6913581-D0CF-46F5-9753-4FD13A428406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="2" r:id="rId1"/>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t>Create the REST Endpoints for the CRUD operations</t>
-  </si>
-  <si>
-    <t>Follow the TDD approach to creating the back end tier. You will still be writing the test cases using JUnit but using the framework support in Spring Boot. You need to cover unit tests that can run in isolation as well as integration tests that will bootstrap Spring context before executing tests.</t>
   </si>
   <si>
     <r>
@@ -371,9 +368,6 @@
     <t>Compile and package the application</t>
   </si>
   <si>
-    <t>Run the JUnit tests and publish the results</t>
-  </si>
-  <si>
     <t>Build executed successfully in Jenkins with passing test cases</t>
   </si>
   <si>
@@ -458,9 +452,6 @@
     <t>Unit and BDD test reports available in Jenkins and SonarQube</t>
   </si>
   <si>
-    <t xml:space="preserve">Add a stage to the pipeline to do a Performance Test with Jmeter and publish the results. </t>
-  </si>
-  <si>
     <t>Do a performance analysis of the  application for 3000 users. Check that the system satisfies the NFRs and SLAs in the Conceptual Problem Statement.</t>
   </si>
   <si>
@@ -548,9 +539,6 @@
     <t>Create the Jenkins Pipeline for ReactJs app</t>
   </si>
   <si>
-    <t>index.html shoul render when hitting the AWS S3 URL</t>
-  </si>
-  <si>
     <t xml:space="preserve">Add a stage to the pipeline to start/restart an AWS EC2 instance. </t>
   </si>
   <si>
@@ -570,9 +558,6 @@
   </si>
   <si>
     <t>Create the Frontend  for the BMS using React and Dockerize the application. Deploy the Spring Boot and ReactJs app to Amazon Web Services.</t>
-  </si>
-  <si>
-    <t>Follow TDD with Jest to build the complete the front end using React, HTML5  and CSS3. Structure your React application according to the Atomic Design Pattern: atoms &gt; molecules &gt; organisms &gt; templates &gt; pages</t>
   </si>
   <si>
     <t>Task 7</t>
@@ -744,17 +729,46 @@
   <si>
     <t>UML model project uploaded to BitBucket  repo in pdf format.</t>
   </si>
+  <si>
+    <t>Follow the TDD approach to creating the back end tier. You will  be writing the test cases using the framework support in Spring Boot. You need to cover unit tests that can run in isolation as well as integration tests that will bootstrap Spring context before executing tests.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add a stage to the pipeline to do a Performance Test with JMeter and publish the results. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow TDD with Jest to build the complete the front end using React, HTML5  and CSS3. </t>
+  </si>
+  <si>
+    <t>Run the Unit tests and publish the results</t>
+  </si>
+  <si>
+    <t>index.html shoul render when hitting the AWS S3 URL. Unit, BDD and Jmeter performance reports generated and available in BitBucket for ReactJS app.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -884,30 +898,27 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -915,64 +926,73 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1255,7 +1275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -1289,7 +1309,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1334,7 +1354,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -1367,27 +1387,27 @@
     </row>
     <row r="8" spans="1:13">
       <c r="B8" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="B9" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="B12" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1395,7 +1415,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -1428,27 +1448,27 @@
     </row>
     <row r="15" spans="1:13">
       <c r="B15" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="B17" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="B18" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="B19" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1456,7 +1476,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -1473,7 +1493,7 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1543,7 +1563,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -1560,7 +1580,7 @@
         <v>19</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1579,7 +1599,7 @@
         <v>8</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -1645,7 +1665,7 @@
         <v>22</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1865,7 +1885,7 @@
         <v>59</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -2027,7 +2047,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -2045,7 +2065,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -2063,7 +2083,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -2081,7 +2101,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -2231,7 +2251,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -2279,7 +2299,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2469,7 +2489,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -2673,7 +2693,7 @@
     <row r="23" spans="1:12">
       <c r="A23" s="2"/>
       <c r="B23" s="12" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -2725,7 +2745,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -2789,7 +2809,7 @@
         <v>8</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -2824,7 +2844,7 @@
         <v>59</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2904,8 +2924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -2938,7 +2958,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2987,7 +3007,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -3082,7 +3102,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -3100,7 +3120,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
@@ -3118,7 +3138,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -3136,7 +3156,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -3151,10 +3171,10 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>69</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>70</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -3169,10 +3189,10 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>71</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>72</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -3187,10 +3207,10 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>74</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -3208,7 +3228,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -3226,7 +3246,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -3248,7 +3268,7 @@
         <v>8</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -3266,7 +3286,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
@@ -3284,7 +3304,7 @@
         <v>11</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
@@ -3302,7 +3322,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -3317,10 +3337,10 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -3335,10 +3355,10 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -3353,10 +3373,10 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
@@ -3371,7 +3391,7 @@
     </row>
     <row r="31" spans="1:12">
       <c r="B31" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -3389,7 +3409,7 @@
         <v>14</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
@@ -3404,7 +3424,7 @@
     <row r="33" spans="1:12">
       <c r="A33" s="2"/>
       <c r="B33" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -3419,7 +3439,7 @@
     <row r="34" spans="1:12">
       <c r="A34" s="2"/>
       <c r="B34" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -3434,7 +3454,7 @@
     <row r="35" spans="1:12">
       <c r="A35" s="2"/>
       <c r="B35" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -3486,7 +3506,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
@@ -3521,7 +3541,7 @@
         <v>28</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -3609,8 +3629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A216D230-190F-4C25-9C3F-8A47CE3732B4}">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q58" sqref="Q58"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -3624,7 +3644,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -3643,7 +3663,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -3667,7 +3687,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
@@ -3692,7 +3712,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -3710,7 +3730,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -3728,7 +3748,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="27"/>
@@ -3760,7 +3780,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -3775,10 +3795,10 @@
     </row>
     <row r="11" spans="1:13" ht="28.95" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -3793,10 +3813,10 @@
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -3811,10 +3831,10 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -3829,10 +3849,10 @@
     </row>
     <row r="14" spans="1:13" ht="36" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -3847,10 +3867,10 @@
     </row>
     <row r="15" spans="1:13" ht="37.950000000000003" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -3865,10 +3885,10 @@
     </row>
     <row r="16" spans="1:13" s="9" customFormat="1" ht="28.95" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="29"/>
@@ -3883,10 +3903,10 @@
     </row>
     <row r="17" spans="1:12" ht="37.950000000000003" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -3901,10 +3921,10 @@
     </row>
     <row r="18" spans="1:12" ht="19.05" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -3922,7 +3942,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -3939,7 +3959,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -3963,7 +3983,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
@@ -3981,7 +4001,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -3999,7 +4019,7 @@
         <v>14</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -4031,7 +4051,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -4063,7 +4083,7 @@
         <v>8</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
@@ -4081,7 +4101,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
@@ -4099,7 +4119,7 @@
         <v>14</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
@@ -4130,7 +4150,7 @@
         <v>22</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -4162,7 +4182,7 @@
         <v>8</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
@@ -4179,8 +4199,8 @@
       <c r="A36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="28" t="s">
-        <v>140</v>
+      <c r="B36" s="31" t="s">
+        <v>136</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
@@ -4193,12 +4213,12 @@
       <c r="K36" s="18"/>
       <c r="L36" s="18"/>
     </row>
-    <row r="37" spans="1:12" ht="14.4" customHeight="1">
+    <row r="37" spans="1:12" ht="28.2" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="28" t="s">
-        <v>136</v>
+      <c r="B37" s="32" t="s">
+        <v>154</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -4230,7 +4250,7 @@
         <v>28</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C39" s="16"/>
       <c r="D39" s="16"/>
@@ -4254,7 +4274,7 @@
         <v>8</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
@@ -4272,7 +4292,7 @@
         <v>9</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
@@ -4290,7 +4310,7 @@
         <v>11</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
@@ -4308,7 +4328,7 @@
         <v>14</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
@@ -4437,7 +4457,7 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>40</v>
@@ -4462,7 +4482,7 @@
         <v>8</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
@@ -4494,10 +4514,10 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:12">

</xml_diff>